<commit_message>
Remove test cats and update Features
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
   <si>
     <t>Feature</t>
   </si>
@@ -668,7 +668,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,7 +938,9 @@
       <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="8"/>
+      <c r="E14" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added features to doc
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="94">
   <si>
     <t>Feature</t>
   </si>
@@ -262,6 +262,45 @@
   </si>
   <si>
     <t>User can add an API to the search</t>
+  </si>
+  <si>
+    <t>Zoom to mouse location</t>
+  </si>
+  <si>
+    <t>Auto Arrange 1</t>
+  </si>
+  <si>
+    <t>Create new window close to source window</t>
+  </si>
+  <si>
+    <t>Auto Arrange 2</t>
+  </si>
+  <si>
+    <t>Auto Arrange 3</t>
+  </si>
+  <si>
+    <t>Create new window in unused space close to source window</t>
+  </si>
+  <si>
+    <t>move other windows to create space for a new window</t>
+  </si>
+  <si>
+    <t>Auto Arrange 4</t>
+  </si>
+  <si>
+    <t>proximity determined by link relevance</t>
+  </si>
+  <si>
+    <t>Window Focus 2</t>
+  </si>
+  <si>
+    <t>Window Focus 1</t>
+  </si>
+  <si>
+    <t>Linked window's size determined by relevance</t>
+  </si>
+  <si>
+    <t>special attribute for a window under focus</t>
   </si>
 </sst>
 </file>
@@ -285,7 +324,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,6 +352,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -344,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -361,6 +406,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,10 +711,10 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,7 +886,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="5"/>
@@ -925,7 +971,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -943,69 +989,67 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>61</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E15" s="8"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E16" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>74</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>37</v>
@@ -1015,13 +1059,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>37</v>
@@ -1031,13 +1075,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>37</v>
@@ -1047,234 +1091,292 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>29</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="5"/>
+      <c r="E23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>70</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>71</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="5"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>27</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="8"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="8"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="8"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="8"/>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="8"/>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="8"/>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="8"/>
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1351,8 +1453,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F30">
-    <sortState ref="A2:F30">
-      <sortCondition ref="D1:D30"/>
+    <sortState ref="A2:F31">
+      <sortCondition ref="A1:A30"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check for window overlap n=8
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -7,19 +7,19 @@
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Features" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Features!$A$1:$F$30</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="96">
   <si>
     <t>Feature</t>
   </si>
@@ -301,6 +301,12 @@
   </si>
   <si>
     <t>special attribute for a window under focus</t>
+  </si>
+  <si>
+    <t>Auto Arrange 5</t>
+  </si>
+  <si>
+    <t>Apply zoom distances to spacing</t>
   </si>
 </sst>
 </file>
@@ -708,13 +714,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,13 +755,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -785,13 +791,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
@@ -803,13 +809,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
@@ -839,13 +845,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>16</v>
@@ -853,7 +859,9 @@
       <c r="E7" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -875,71 +883,73 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>64</v>
+      <c r="E11" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>16</v>
@@ -947,19 +957,17 @@
       <c r="E12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>16</v>
@@ -967,73 +975,73 @@
       <c r="E13" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>74</v>
-      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>37</v>
@@ -1043,45 +1051,49 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="8"/>
+      <c r="E18" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>40</v>
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="8"/>
+      <c r="E19" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>37</v>
@@ -1089,45 +1101,37 @@
       <c r="E20" s="8"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>70</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>71</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -1151,115 +1155,109 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>61</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E29" s="8"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>37</v>
@@ -1285,107 +1283,127 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="5"/>
+      <c r="A38" s="2">
+        <v>27</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
@@ -1451,10 +1469,18 @@
       <c r="E46" s="2"/>
       <c r="F46" s="5"/>
     </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="5"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F30">
-    <sortState ref="A2:F31">
-      <sortCondition ref="A1:A30"/>
+    <sortState ref="A2:F38">
+      <sortCondition ref="D1:D30"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enter Key + features
Enter key support for search.  Added bugs section to features doc
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Bugs-Tweaks" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Bugs-Tweaks'!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Features!$A$1:$F$30</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="131">
   <si>
     <t>Feature</t>
   </si>
@@ -264,9 +264,6 @@
     <t>User can add an API to the search</t>
   </si>
   <si>
-    <t>Zoom to mouse location</t>
-  </si>
-  <si>
     <t>Auto Arrange 1</t>
   </si>
   <si>
@@ -310,6 +307,111 @@
   </si>
   <si>
     <t>Draggable background</t>
+  </si>
+  <si>
+    <t>Zoom Spacing</t>
+  </si>
+  <si>
+    <t>Bug/Tweak</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Zoom to Mouse</t>
+  </si>
+  <si>
+    <t>Space between windows is not maintained properly on zoom</t>
+  </si>
+  <si>
+    <t>Zoom should centre the screen on the mouse location</t>
+  </si>
+  <si>
+    <t>Drag background on Firefox</t>
+  </si>
+  <si>
+    <t>does not work</t>
+  </si>
+  <si>
+    <t>Grid arrange</t>
+  </si>
+  <si>
+    <t>Enter button search</t>
+  </si>
+  <si>
+    <t>Enter button should execute the search (not refresh page)</t>
+  </si>
+  <si>
+    <t>Background Drag does not refresh all links</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Zoom does not refresh all links</t>
+  </si>
+  <si>
+    <t>Add external link to Wikipedia article</t>
+  </si>
+  <si>
+    <t>at the end of the summary section</t>
+  </si>
+  <si>
+    <t>Filter out "coordinates" as a non-valid first paragraph</t>
+  </si>
+  <si>
+    <t>Articles with a coordinate will only show the lat/lon in the summary</t>
+  </si>
+  <si>
+    <t>ex: Hong Kong</t>
+  </si>
+  <si>
+    <t>Some articles contain that sentence at the end of the summary</t>
+  </si>
+  <si>
+    <t>Some hyperlinks in the summary do not draw the line when clicked</t>
+  </si>
+  <si>
+    <t>ex: Bear -&gt; Asia</t>
+  </si>
+  <si>
+    <t>New windows should start in Display2 (image) when zoomed out</t>
+  </si>
+  <si>
+    <t>Filter out "Cite error: there are &lt;ref&gt; tags..." at the end of the summary</t>
+  </si>
+  <si>
+    <t>Handle redirected articles</t>
+  </si>
+  <si>
+    <t>If an article has a redirect, open the redirect instead</t>
+  </si>
+  <si>
+    <t>ex: Audio Recording</t>
+  </si>
+  <si>
+    <t>Browser window should not have scroll bars for off screen content</t>
+  </si>
+  <si>
+    <t>Titles spill past the window when zoomed out</t>
+  </si>
+  <si>
+    <t>Wrap/split long words or shrink font</t>
+  </si>
+  <si>
+    <t>Change mouse icon on background drag</t>
+  </si>
+  <si>
+    <t>check event variable (pageX vs clientX)</t>
+  </si>
+  <si>
+    <t>ex: Sound, Hat</t>
+  </si>
+  <si>
+    <t>partial</t>
+  </si>
+  <si>
+    <t>works while clicked inside the text box</t>
   </si>
 </sst>
 </file>
@@ -420,7 +522,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -717,13 +841,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,18 +1173,22 @@
       <c r="D17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="5"/>
+      <c r="E17" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>37</v>
@@ -1075,10 +1203,10 @@
         <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>37</v>
@@ -1093,10 +1221,10 @@
         <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>37</v>
@@ -1109,10 +1237,10 @@
         <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>37</v>
@@ -1125,10 +1253,10 @@
         <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>37</v>
@@ -1225,10 +1353,10 @@
         <v>36</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>37</v>
@@ -1241,10 +1369,10 @@
         <v>35</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>37</v>
@@ -1270,29 +1398,33 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>46</v>
@@ -1301,35 +1433,31 @@
         <v>65</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>71</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>26</v>
@@ -1342,88 +1470,80 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>73</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>38</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1481,14 +1601,6 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="5"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F30">
@@ -1502,24 +1614,280 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35" style="5" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14" style="2" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E1"/>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"open"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"partial"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Citer Error + Browser scroll
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -9,17 +9,19 @@
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
     <sheet name="Bugs-Tweaks" sheetId="2" r:id="rId2"/>
+    <sheet name="MetaData" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Bugs-Tweaks'!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Features!$A$1:$F$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MetaData!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="157">
   <si>
     <t>Feature</t>
   </si>
@@ -412,6 +414,84 @@
   </si>
   <si>
     <t>works while clicked inside the text box</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Genres</t>
+  </si>
+  <si>
+    <t>Info Box text</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Years active</t>
+  </si>
+  <si>
+    <t>Labels</t>
+  </si>
+  <si>
+    <t>Members</t>
+  </si>
+  <si>
+    <t>Associated acts</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Past members</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Born</t>
+  </si>
+  <si>
+    <t>Born (date)</t>
+  </si>
+  <si>
+    <t>Died (date)</t>
+  </si>
+  <si>
+    <t>Died</t>
+  </si>
+  <si>
+    <t>Notable works</t>
+  </si>
+  <si>
+    <t>Notable work(s)</t>
+  </si>
+  <si>
+    <t>ex painting, sculpting</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Movement</t>
   </si>
 </sst>
 </file>
@@ -500,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -518,11 +598,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -541,6 +625,27 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -847,7 +952,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,7 +1725,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,8 +1885,8 @@
       <c r="C10" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>98</v>
+      <c r="D10" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>128</v>
@@ -1845,8 +1950,8 @@
       <c r="C14" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>98</v>
+      <c r="D14" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1880,14 +1985,356 @@
   </sheetData>
   <autoFilter ref="A1:E1"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"partial"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"open"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"partial"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G1"/>
+  <conditionalFormatting sqref="F1:F15">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"partial"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
background mouse drag + grid on zoom
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="158">
   <si>
     <t>Feature</t>
   </si>
@@ -492,6 +492,9 @@
   </si>
   <si>
     <t>Movement</t>
+  </si>
+  <si>
+    <t>new windows start with links and summary closed</t>
   </si>
 </sst>
 </file>
@@ -606,7 +609,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -949,7 +980,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
@@ -1725,7 +1756,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1919,8 +1950,11 @@
       <c r="C12" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>98</v>
+      <c r="D12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1978,17 +2012,17 @@
       <c r="C16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>98</v>
+      <c r="D16" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2328,10 +2362,10 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="F1:F15">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
redirects! + date parse bugs
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
     <sheet name="Bugs-Tweaks" sheetId="2" r:id="rId2"/>
     <sheet name="MetaData" sheetId="3" r:id="rId3"/>
+    <sheet name="Date format" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Bugs-Tweaks'!$A$1:$E$1</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="183">
   <si>
     <t>Feature</t>
   </si>
@@ -516,6 +517,60 @@
   </si>
   <si>
     <t>Publisher</t>
+  </si>
+  <si>
+    <t>Dates &lt; 1000 CE</t>
+  </si>
+  <si>
+    <t>do not sort</t>
+  </si>
+  <si>
+    <t>bday tag</t>
+  </si>
+  <si>
+    <t>dday tag</t>
+  </si>
+  <si>
+    <t>"April 15, 2011"</t>
+  </si>
+  <si>
+    <t>Month dd, yyyy</t>
+  </si>
+  <si>
+    <t>"before 31 October 1451"</t>
+  </si>
+  <si>
+    <t>"31 October 1451"</t>
+  </si>
+  <si>
+    <t>"c. 1500"</t>
+  </si>
+  <si>
+    <t>"20 May 1506 (aged c. 54)"</t>
+  </si>
+  <si>
+    <t>"20 May 1506 City"</t>
+  </si>
+  <si>
+    <t>"20 May 1506, City"</t>
+  </si>
+  <si>
+    <t>"1254 city"</t>
+  </si>
+  <si>
+    <t>"ca. 1455"</t>
+  </si>
+  <si>
+    <t>Marco Polo</t>
+  </si>
+  <si>
+    <t>"20-21 May 1506 City"</t>
+  </si>
+  <si>
+    <t>Filipa Moniz Perestrelo</t>
+  </si>
+  <si>
+    <t>Christopher Columbus</t>
   </si>
 </sst>
 </file>
@@ -645,7 +700,161 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1842,13 +2051,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,8 +2268,8 @@
       <c r="C13" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>98</v>
+      <c r="D13" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>122</v>
@@ -2108,13 +2317,27 @@
         <v>61</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2127,8 +2350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,7 +2424,7 @@
         <v>146</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -2426,7 +2649,7 @@
         <v>146</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="G14" s="2"/>
     </row>
@@ -2447,7 +2670,7 @@
         <v>146</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="G15" s="2"/>
     </row>
@@ -2461,8 +2684,11 @@
       <c r="D16" s="14" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
         <v>156</v>
       </c>
@@ -2473,7 +2699,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
         <v>156</v>
       </c>
@@ -2484,7 +2710,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>156</v>
       </c>
@@ -2494,8 +2720,11 @@
       <c r="D19" s="14" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>161</v>
       </c>
@@ -2506,7 +2735,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
         <v>161</v>
       </c>
@@ -2516,8 +2745,11 @@
       <c r="D21" s="14" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
         <v>161</v>
       </c>
@@ -2530,70 +2762,249 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G1"/>
-  <conditionalFormatting sqref="F1 F13:F15 F6 F3 F9">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+  <conditionalFormatting sqref="F1 F13 F6 F9">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F8">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+      <formula>"open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>"partial"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>"open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14:F15">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+      <formula>"partial"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>"open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"partial"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"partial"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"partial"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>176</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed enter key on search
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -700,7 +700,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="44">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2057,7 +2085,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2186,8 +2214,8 @@
       <c r="C8" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>98</v>
+      <c r="D8" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2200,8 +2228,8 @@
       <c r="C9" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>98</v>
+      <c r="D9" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>114</v>
@@ -2334,10 +2362,10 @@
   </sheetData>
   <autoFilter ref="A1:E1"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2763,106 +2791,106 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="F1 F13 F6 F9">
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="25" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F8">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F15">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>